<commit_message>
phase shift sensor modelling
</commit_message>
<xml_diff>
--- a/teensy4theremin/kicad/teensy4_pins_layout.xlsx
+++ b/teensy4theremin/kicad/teensy4_pins_layout.xlsx
@@ -17,6 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="174">
   <si>
     <t>GND</t>
   </si>
@@ -509,6 +510,48 @@
   <si>
     <t>116V</t>
   </si>
+  <si>
+    <t>1.5mH</t>
+  </si>
+  <si>
+    <t>180V</t>
+  </si>
+  <si>
+    <t>0.1mm*31mm winding</t>
+  </si>
+  <si>
+    <t>Cbuf=2.2/3 pf, Cpar = 3.3/3 pf</t>
+  </si>
+  <si>
+    <t>Cbuf=2.2/3 pf, Cpar = 6.8/3 pf</t>
+  </si>
+  <si>
+    <t>single inv 5V, Cfeed=0.1uF</t>
+  </si>
+  <si>
+    <t>Cbuf=2.2/3 pf, Cpar = 0 pf</t>
+  </si>
+  <si>
+    <t>single inv 5V, feed = R0</t>
+  </si>
+  <si>
+    <t>single inv 5V, feed = 0.1uF</t>
+  </si>
+  <si>
+    <t>186V</t>
+  </si>
+  <si>
+    <t>2.5mH</t>
+  </si>
+  <si>
+    <t>2mH</t>
+  </si>
+  <si>
+    <t>1.8mH</t>
+  </si>
+  <si>
+    <t>1mH</t>
+  </si>
 </sst>
 </file>
 
@@ -519,7 +562,7 @@
     <numFmt numFmtId="165" formatCode="0.00000000"/>
     <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -527,8 +570,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,6 +623,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -599,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -633,6 +691,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -22370,8 +22436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:W111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R10" sqref="R10:W109"/>
+    <sheetView topLeftCell="B70" workbookViewId="0">
+      <selection activeCell="U93" sqref="U93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25268,8 +25334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AL747"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145:I145"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J77" sqref="J77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25278,7 +25344,7 @@
     <col min="5" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.7109375" customWidth="1"/>
     <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" customWidth="1"/>
     <col min="16" max="16" width="10.5703125" customWidth="1"/>
     <col min="18" max="18" width="14.5703125" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
@@ -28780,11 +28846,11 @@
         <f t="shared" si="18"/>
         <v>76</v>
       </c>
-      <c r="H79" s="16">
+      <c r="H79" s="21">
         <f t="shared" si="19"/>
         <v>3.8000000000000001E-7</v>
       </c>
-      <c r="I79" s="16">
+      <c r="I79" s="21">
         <f t="shared" si="20"/>
         <v>7.6000000000000003E-7</v>
       </c>
@@ -28870,11 +28936,11 @@
         <f t="shared" si="18"/>
         <v>77</v>
       </c>
-      <c r="H82" s="16">
+      <c r="H82" s="22">
         <f t="shared" si="19"/>
         <v>3.8500000000000002E-7</v>
       </c>
-      <c r="I82" s="16">
+      <c r="I82" s="22">
         <f t="shared" si="20"/>
         <v>7.750000000000001E-7</v>
       </c>
@@ -29106,6 +29172,9 @@
         <f t="shared" si="20"/>
         <v>7.9999999999999996E-7</v>
       </c>
+      <c r="K87">
+        <v>131</v>
+      </c>
       <c r="N87">
         <v>0.5</v>
       </c>
@@ -29149,6 +29218,9 @@
         <f t="shared" si="20"/>
         <v>8.0500000000000002E-7</v>
       </c>
+      <c r="K88">
+        <v>116</v>
+      </c>
       <c r="N88">
         <v>0.6</v>
       </c>
@@ -29199,6 +29271,9 @@
         <f t="shared" si="20"/>
         <v>8.0999999999999997E-7</v>
       </c>
+      <c r="K89">
+        <v>87</v>
+      </c>
       <c r="N89">
         <v>0.7</v>
       </c>
@@ -29297,6 +29372,9 @@
         <f t="shared" si="20"/>
         <v>8.1999999999999998E-7</v>
       </c>
+      <c r="K91">
+        <v>51</v>
+      </c>
       <c r="N91">
         <v>0.9</v>
       </c>
@@ -29377,6 +29455,9 @@
         <f t="shared" si="20"/>
         <v>8.300000000000001E-7</v>
       </c>
+      <c r="K93">
+        <v>35</v>
+      </c>
       <c r="N93">
         <v>1.1000000000000001</v>
       </c>
@@ -30830,7 +30911,7 @@
         <f t="shared" si="19"/>
         <v>4.8999999999999997E-7</v>
       </c>
-      <c r="I124" s="16">
+      <c r="I124" s="21">
         <f t="shared" si="20"/>
         <v>9.850000000000001E-7</v>
       </c>
@@ -39121,6 +39202,38 @@
         <f t="shared" si="46"/>
         <v>2.03E-6</v>
       </c>
+      <c r="N333" t="s">
+        <v>165</v>
+      </c>
+      <c r="O333" t="s">
+        <v>160</v>
+      </c>
+      <c r="P333" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q333" t="s">
+        <v>117</v>
+      </c>
+      <c r="R333" t="s">
+        <v>163</v>
+      </c>
+      <c r="S333">
+        <v>1.6839999999999999</v>
+      </c>
+      <c r="T333">
+        <v>2.484</v>
+      </c>
+      <c r="U333">
+        <f>T333-S333</f>
+        <v>0.8</v>
+      </c>
+      <c r="V333">
+        <f>1/U333</f>
+        <v>1.25</v>
+      </c>
+      <c r="W333" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="334" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C334">
@@ -39150,6 +39263,19 @@
         <f t="shared" si="46"/>
         <v>2.035E-6</v>
       </c>
+      <c r="N334" t="s">
+        <v>162</v>
+      </c>
+      <c r="S334">
+        <v>1.6843999999999999</v>
+      </c>
+      <c r="T334">
+        <v>1.7035</v>
+      </c>
+      <c r="U334">
+        <f>T334-S334</f>
+        <v>1.9100000000000117E-2</v>
+      </c>
     </row>
     <row r="335" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C335">
@@ -39179,6 +39305,18 @@
         <f t="shared" si="46"/>
         <v>2.04E-6</v>
       </c>
+      <c r="U335">
+        <f>U334/U333</f>
+        <v>2.3875000000000146E-2</v>
+      </c>
+      <c r="V335">
+        <f>U335*4</f>
+        <v>9.5500000000000584E-2</v>
+      </c>
+      <c r="W335">
+        <f>1/U335</f>
+        <v>41.884816753926444</v>
+      </c>
     </row>
     <row r="336" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C336">
@@ -39209,7 +39347,7 @@
         <v>2.0449999999999999E-6</v>
       </c>
     </row>
-    <row r="337" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C337">
         <v>410</v>
       </c>
@@ -39237,8 +39375,40 @@
         <f t="shared" si="46"/>
         <v>2.0499999999999999E-6</v>
       </c>
-    </row>
-    <row r="338" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N337" t="s">
+        <v>165</v>
+      </c>
+      <c r="O337" t="s">
+        <v>160</v>
+      </c>
+      <c r="P337" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q337" t="s">
+        <v>117</v>
+      </c>
+      <c r="R337" t="s">
+        <v>164</v>
+      </c>
+      <c r="S337">
+        <v>1.7158</v>
+      </c>
+      <c r="T337">
+        <v>2.5606</v>
+      </c>
+      <c r="U337">
+        <f>T337-S337</f>
+        <v>0.8448</v>
+      </c>
+      <c r="V337">
+        <f>1/U337</f>
+        <v>1.1837121212121213</v>
+      </c>
+      <c r="W337" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="338" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C338">
         <v>411</v>
       </c>
@@ -39266,8 +39436,21 @@
         <f t="shared" si="46"/>
         <v>2.0549999999999998E-6</v>
       </c>
-    </row>
-    <row r="339" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N338" t="s">
+        <v>162</v>
+      </c>
+      <c r="S338">
+        <v>1.74027</v>
+      </c>
+      <c r="T338">
+        <v>1.75379</v>
+      </c>
+      <c r="U338">
+        <f>T338-S338</f>
+        <v>1.3519999999999976E-2</v>
+      </c>
+    </row>
+    <row r="339" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C339">
         <v>412</v>
       </c>
@@ -39295,8 +39478,20 @@
         <f t="shared" si="46"/>
         <v>2.0600000000000002E-6</v>
       </c>
-    </row>
-    <row r="340" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="U339">
+        <f>U338/U337</f>
+        <v>1.600378787878785E-2</v>
+      </c>
+      <c r="V339">
+        <f>U339*4</f>
+        <v>6.40151515151514E-2</v>
+      </c>
+      <c r="W339">
+        <f>1/U339</f>
+        <v>62.485207100591829</v>
+      </c>
+    </row>
+    <row r="340" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C340">
         <v>413</v>
       </c>
@@ -39325,7 +39520,7 @@
         <v>2.0650000000000001E-6</v>
       </c>
     </row>
-    <row r="341" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="341" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C341">
         <v>414</v>
       </c>
@@ -39353,8 +39548,40 @@
         <f t="shared" si="46"/>
         <v>2.0700000000000001E-6</v>
       </c>
-    </row>
-    <row r="342" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N341" t="s">
+        <v>165</v>
+      </c>
+      <c r="O341" t="s">
+        <v>160</v>
+      </c>
+      <c r="P341" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q341" t="s">
+        <v>117</v>
+      </c>
+      <c r="R341" t="s">
+        <v>166</v>
+      </c>
+      <c r="S341">
+        <v>1.3955</v>
+      </c>
+      <c r="T341">
+        <v>2.1554000000000002</v>
+      </c>
+      <c r="U341">
+        <f>T341-S341</f>
+        <v>0.75990000000000024</v>
+      </c>
+      <c r="V341">
+        <f>1/U341</f>
+        <v>1.3159626266614024</v>
+      </c>
+      <c r="W341" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="342" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C342">
         <v>415</v>
       </c>
@@ -39382,8 +39609,21 @@
         <f t="shared" si="46"/>
         <v>2.075E-6</v>
       </c>
-    </row>
-    <row r="343" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N342" t="s">
+        <v>162</v>
+      </c>
+      <c r="S342">
+        <v>1.80742</v>
+      </c>
+      <c r="T342">
+        <v>1.8229</v>
+      </c>
+      <c r="U342">
+        <f>T342-S342</f>
+        <v>1.5479999999999938E-2</v>
+      </c>
+    </row>
+    <row r="343" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C343">
         <v>416</v>
       </c>
@@ -39411,8 +39651,20 @@
         <f t="shared" si="46"/>
         <v>2.08E-6</v>
       </c>
-    </row>
-    <row r="344" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="U343">
+        <f>U342/U341</f>
+        <v>2.0371101460718428E-2</v>
+      </c>
+      <c r="V343">
+        <f>U343*4</f>
+        <v>8.1484405842873711E-2</v>
+      </c>
+      <c r="W343">
+        <f>1/U343</f>
+        <v>49.08914728682192</v>
+      </c>
+    </row>
+    <row r="344" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C344">
         <v>417</v>
       </c>
@@ -39441,7 +39693,7 @@
         <v>2.0849999999999999E-6</v>
       </c>
     </row>
-    <row r="345" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="345" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C345">
         <v>418</v>
       </c>
@@ -39469,8 +39721,40 @@
         <f t="shared" si="46"/>
         <v>2.0900000000000003E-6</v>
       </c>
-    </row>
-    <row r="346" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N345" t="s">
+        <v>165</v>
+      </c>
+      <c r="O345" t="s">
+        <v>160</v>
+      </c>
+      <c r="P345" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q345" t="s">
+        <v>117</v>
+      </c>
+      <c r="R345" t="s">
+        <v>166</v>
+      </c>
+      <c r="S345">
+        <v>1.7049000000000001</v>
+      </c>
+      <c r="T345">
+        <v>2.4601999999999999</v>
+      </c>
+      <c r="U345">
+        <f>T345-S345</f>
+        <v>0.75529999999999986</v>
+      </c>
+      <c r="V345">
+        <f>1/U345</f>
+        <v>1.3239772275916857</v>
+      </c>
+      <c r="W345" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="346" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C346">
         <v>419</v>
       </c>
@@ -39498,8 +39782,21 @@
         <f t="shared" si="46"/>
         <v>2.0950000000000003E-6</v>
       </c>
-    </row>
-    <row r="347" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N346" t="s">
+        <v>162</v>
+      </c>
+      <c r="S346">
+        <v>1.7048000000000001</v>
+      </c>
+      <c r="T346">
+        <v>1.7181</v>
+      </c>
+      <c r="U346">
+        <f>T346-S346</f>
+        <v>1.3299999999999867E-2</v>
+      </c>
+    </row>
+    <row r="347" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C347">
         <v>420</v>
       </c>
@@ -39527,8 +39824,20 @@
         <f t="shared" si="46"/>
         <v>2.0999999999999998E-6</v>
       </c>
-    </row>
-    <row r="348" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="U347">
+        <f>U346/U345</f>
+        <v>1.7608897126969243E-2</v>
+      </c>
+      <c r="V347">
+        <f>U347*4</f>
+        <v>7.043558850787697E-2</v>
+      </c>
+      <c r="W347">
+        <f>1/U347</f>
+        <v>56.789473684211089</v>
+      </c>
+    </row>
+    <row r="348" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C348">
         <v>421</v>
       </c>
@@ -39557,7 +39866,7 @@
         <v>2.1050000000000002E-6</v>
       </c>
     </row>
-    <row r="349" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C349">
         <v>422</v>
       </c>
@@ -39585,8 +39894,40 @@
         <f t="shared" si="46"/>
         <v>2.1100000000000001E-6</v>
       </c>
-    </row>
-    <row r="350" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N349" t="s">
+        <v>167</v>
+      </c>
+      <c r="O349" t="s">
+        <v>160</v>
+      </c>
+      <c r="P349" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q349" t="s">
+        <v>117</v>
+      </c>
+      <c r="R349" t="s">
+        <v>163</v>
+      </c>
+      <c r="S349">
+        <v>1.5640000000000001</v>
+      </c>
+      <c r="T349">
+        <v>2.3490000000000002</v>
+      </c>
+      <c r="U349">
+        <f>T349-S349</f>
+        <v>0.78500000000000014</v>
+      </c>
+      <c r="V349">
+        <f>1/U349</f>
+        <v>1.2738853503184711</v>
+      </c>
+      <c r="W349" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="350" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C350">
         <v>423</v>
       </c>
@@ -39614,8 +39955,21 @@
         <f t="shared" si="46"/>
         <v>2.1150000000000001E-6</v>
       </c>
-    </row>
-    <row r="351" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N350" t="s">
+        <v>162</v>
+      </c>
+      <c r="S350">
+        <v>1.5642799999999999</v>
+      </c>
+      <c r="T350">
+        <v>1.5778000000000001</v>
+      </c>
+      <c r="U350">
+        <f>T350-S350</f>
+        <v>1.3520000000000199E-2</v>
+      </c>
+    </row>
+    <row r="351" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C351">
         <v>424</v>
       </c>
@@ -39643,8 +39997,20 @@
         <f t="shared" si="46"/>
         <v>2.12E-6</v>
       </c>
-    </row>
-    <row r="352" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="U351">
+        <f>U350/U349</f>
+        <v>1.7222929936305982E-2</v>
+      </c>
+      <c r="V351">
+        <f>U351*4</f>
+        <v>6.8891719745223928E-2</v>
+      </c>
+      <c r="W351">
+        <f>1/U351</f>
+        <v>58.06213017751395</v>
+      </c>
+    </row>
+    <row r="352" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C352">
         <v>425</v>
       </c>
@@ -39673,7 +40039,7 @@
         <v>2.125E-6</v>
       </c>
     </row>
-    <row r="353" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="353" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C353">
         <v>426</v>
       </c>
@@ -39701,8 +40067,40 @@
         <f t="shared" si="46"/>
         <v>2.1299999999999999E-6</v>
       </c>
-    </row>
-    <row r="354" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N353" t="s">
+        <v>167</v>
+      </c>
+      <c r="O353" t="s">
+        <v>160</v>
+      </c>
+      <c r="P353" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q353" t="s">
+        <v>117</v>
+      </c>
+      <c r="R353" t="s">
+        <v>163</v>
+      </c>
+      <c r="S353">
+        <v>1.5640000000000001</v>
+      </c>
+      <c r="T353">
+        <v>2.3490000000000002</v>
+      </c>
+      <c r="U353">
+        <f>T353-S353</f>
+        <v>0.78500000000000014</v>
+      </c>
+      <c r="V353">
+        <f>1/U353</f>
+        <v>1.2738853503184711</v>
+      </c>
+      <c r="W353" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="354" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C354">
         <v>427</v>
       </c>
@@ -39730,8 +40128,21 @@
         <f t="shared" si="46"/>
         <v>2.1349999999999999E-6</v>
       </c>
-    </row>
-    <row r="355" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N354" t="s">
+        <v>162</v>
+      </c>
+      <c r="S354">
+        <v>2.3066900000000001</v>
+      </c>
+      <c r="T354">
+        <v>2.3200699999999999</v>
+      </c>
+      <c r="U354">
+        <f>T354-S354</f>
+        <v>1.3379999999999725E-2</v>
+      </c>
+    </row>
+    <row r="355" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C355">
         <v>428</v>
       </c>
@@ -39759,8 +40170,20 @@
         <f t="shared" si="46"/>
         <v>2.1400000000000003E-6</v>
       </c>
-    </row>
-    <row r="356" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="U355">
+        <f>U354/U353</f>
+        <v>1.7044585987260795E-2</v>
+      </c>
+      <c r="V355">
+        <f>U355*4</f>
+        <v>6.817834394904318E-2</v>
+      </c>
+      <c r="W355">
+        <f>1/U355</f>
+        <v>58.669656203289698</v>
+      </c>
+    </row>
+    <row r="356" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C356">
         <v>429</v>
       </c>
@@ -39789,7 +40212,7 @@
         <v>2.1449999999999998E-6</v>
       </c>
     </row>
-    <row r="357" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="357" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C357">
         <v>430</v>
       </c>
@@ -39817,8 +40240,40 @@
         <f t="shared" si="46"/>
         <v>2.1500000000000002E-6</v>
       </c>
-    </row>
-    <row r="358" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N357" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="O357" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="P357" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q357" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="R357" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="S357" s="19">
+        <v>1.766</v>
+      </c>
+      <c r="T357" s="19">
+        <v>2.5266000000000002</v>
+      </c>
+      <c r="U357" s="19">
+        <f>T357-S357</f>
+        <v>0.76060000000000016</v>
+      </c>
+      <c r="V357" s="19">
+        <f>1/U357</f>
+        <v>1.3147515119642386</v>
+      </c>
+      <c r="W357" s="20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="358" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C358">
         <v>431</v>
       </c>
@@ -39846,8 +40301,21 @@
         <f t="shared" si="46"/>
         <v>2.1550000000000001E-6</v>
       </c>
-    </row>
-    <row r="359" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N358" t="s">
+        <v>162</v>
+      </c>
+      <c r="S358">
+        <v>1.786</v>
+      </c>
+      <c r="T358">
+        <v>1.8069999999999999</v>
+      </c>
+      <c r="U358">
+        <f>T358-S358</f>
+        <v>2.0999999999999908E-2</v>
+      </c>
+    </row>
+    <row r="359" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C359">
         <v>432</v>
       </c>
@@ -39875,8 +40343,26 @@
         <f t="shared" si="46"/>
         <v>2.1600000000000001E-6</v>
       </c>
-    </row>
-    <row r="360" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="S359">
+        <v>1.4014</v>
+      </c>
+      <c r="T359">
+        <v>1.4227000000000001</v>
+      </c>
+      <c r="U359">
+        <f>U358/U357</f>
+        <v>2.7609781751248886E-2</v>
+      </c>
+      <c r="V359">
+        <f>U359*4</f>
+        <v>0.11043912700499554</v>
+      </c>
+      <c r="W359">
+        <f>1/U359</f>
+        <v>36.219047619047785</v>
+      </c>
+    </row>
+    <row r="360" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C360">
         <v>433</v>
       </c>
@@ -39904,8 +40390,12 @@
         <f t="shared" si="46"/>
         <v>2.165E-6</v>
       </c>
-    </row>
-    <row r="361" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="U360">
+        <f>T359-S359</f>
+        <v>2.1300000000000097E-2</v>
+      </c>
+    </row>
+    <row r="361" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C361">
         <v>434</v>
       </c>
@@ -39934,7 +40424,7 @@
         <v>2.17E-6</v>
       </c>
     </row>
-    <row r="362" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="362" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C362">
         <v>435</v>
       </c>
@@ -39962,8 +40452,40 @@
         <f t="shared" si="46"/>
         <v>2.1749999999999999E-6</v>
       </c>
-    </row>
-    <row r="363" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N362" t="s">
+        <v>167</v>
+      </c>
+      <c r="O362" t="s">
+        <v>170</v>
+      </c>
+      <c r="P362" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q362" t="s">
+        <v>117</v>
+      </c>
+      <c r="R362" t="s">
+        <v>166</v>
+      </c>
+      <c r="S362">
+        <v>1.5</v>
+      </c>
+      <c r="T362">
+        <v>2.4849999999999999</v>
+      </c>
+      <c r="U362">
+        <f>T362-S362</f>
+        <v>0.98499999999999988</v>
+      </c>
+      <c r="V362">
+        <f>1/U362</f>
+        <v>1.0152284263959392</v>
+      </c>
+      <c r="W362" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="363" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C363">
         <v>436</v>
       </c>
@@ -39991,8 +40513,21 @@
         <f t="shared" si="46"/>
         <v>2.1799999999999999E-6</v>
       </c>
-    </row>
-    <row r="364" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N363" t="s">
+        <v>162</v>
+      </c>
+      <c r="S363">
+        <v>1.5168999999999999</v>
+      </c>
+      <c r="T363">
+        <v>1.5347</v>
+      </c>
+      <c r="U363">
+        <f>T363-S363</f>
+        <v>1.7800000000000038E-2</v>
+      </c>
+    </row>
+    <row r="364" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C364">
         <v>437</v>
       </c>
@@ -40020,8 +40555,20 @@
         <f t="shared" si="46"/>
         <v>2.1849999999999998E-6</v>
       </c>
-    </row>
-    <row r="365" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="U364">
+        <f>U363/U362</f>
+        <v>1.8071065989847757E-2</v>
+      </c>
+      <c r="V364">
+        <f>U364*4</f>
+        <v>7.2284263959391026E-2</v>
+      </c>
+      <c r="W364">
+        <f>1/U364</f>
+        <v>55.337078651685268</v>
+      </c>
+    </row>
+    <row r="365" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C365">
         <v>438</v>
       </c>
@@ -40050,7 +40597,7 @@
         <v>2.1900000000000002E-6</v>
       </c>
     </row>
-    <row r="366" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="366" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C366">
         <v>439</v>
       </c>
@@ -40078,8 +40625,40 @@
         <f t="shared" si="46"/>
         <v>2.1950000000000002E-6</v>
       </c>
-    </row>
-    <row r="367" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N366" t="s">
+        <v>167</v>
+      </c>
+      <c r="O366" t="s">
+        <v>171</v>
+      </c>
+      <c r="P366" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q366" t="s">
+        <v>117</v>
+      </c>
+      <c r="R366" t="s">
+        <v>166</v>
+      </c>
+      <c r="S366">
+        <v>1.4570000000000001</v>
+      </c>
+      <c r="T366">
+        <v>2.3372999999999999</v>
+      </c>
+      <c r="U366">
+        <f>T366-S366</f>
+        <v>0.88029999999999986</v>
+      </c>
+      <c r="V366">
+        <f>1/U366</f>
+        <v>1.135976371691469</v>
+      </c>
+      <c r="W366" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="367" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C367">
         <v>440</v>
       </c>
@@ -40107,8 +40686,21 @@
         <f t="shared" si="46"/>
         <v>2.2000000000000001E-6</v>
       </c>
-    </row>
-    <row r="368" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N367" t="s">
+        <v>162</v>
+      </c>
+      <c r="S367">
+        <v>1.4886999999999999</v>
+      </c>
+      <c r="T367">
+        <v>1.5059</v>
+      </c>
+      <c r="U367">
+        <f>T367-S367</f>
+        <v>1.7200000000000104E-2</v>
+      </c>
+    </row>
+    <row r="368" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C368">
         <v>441</v>
       </c>
@@ -40136,8 +40728,20 @@
         <f t="shared" si="46"/>
         <v>2.2050000000000001E-6</v>
       </c>
-    </row>
-    <row r="369" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="U368">
+        <f>U367/U366</f>
+        <v>1.9538793593093386E-2</v>
+      </c>
+      <c r="V368">
+        <f>U368*4</f>
+        <v>7.8155174372373543E-2</v>
+      </c>
+      <c r="W368">
+        <f>1/U368</f>
+        <v>51.180232558139217</v>
+      </c>
+    </row>
+    <row r="369" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C369">
         <v>442</v>
       </c>
@@ -40166,7 +40770,7 @@
         <v>2.21E-6</v>
       </c>
     </row>
-    <row r="370" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="370" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C370">
         <v>443</v>
       </c>
@@ -40194,8 +40798,40 @@
         <f t="shared" si="46"/>
         <v>2.215E-6</v>
       </c>
-    </row>
-    <row r="371" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N370" t="s">
+        <v>167</v>
+      </c>
+      <c r="O370" t="s">
+        <v>172</v>
+      </c>
+      <c r="P370" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q370" t="s">
+        <v>117</v>
+      </c>
+      <c r="R370" t="s">
+        <v>166</v>
+      </c>
+      <c r="S370">
+        <v>1.0580000000000001</v>
+      </c>
+      <c r="T370">
+        <v>1.8919999999999999</v>
+      </c>
+      <c r="U370">
+        <f>T370-S370</f>
+        <v>0.83399999999999985</v>
+      </c>
+      <c r="V370">
+        <f>1/U370</f>
+        <v>1.1990407673860914</v>
+      </c>
+      <c r="W370" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="371" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C371">
         <v>444</v>
       </c>
@@ -40223,8 +40859,21 @@
         <f t="shared" si="46"/>
         <v>2.2199999999999999E-6</v>
       </c>
-    </row>
-    <row r="372" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N371" t="s">
+        <v>162</v>
+      </c>
+      <c r="S371">
+        <v>1.1346000000000001</v>
+      </c>
+      <c r="T371">
+        <v>1.1498999999999999</v>
+      </c>
+      <c r="U371">
+        <f>T371-S371</f>
+        <v>1.5299999999999869E-2</v>
+      </c>
+    </row>
+    <row r="372" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C372">
         <v>445</v>
       </c>
@@ -40252,8 +40901,20 @@
         <f t="shared" si="46"/>
         <v>2.2250000000000003E-6</v>
       </c>
-    </row>
-    <row r="373" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="U372">
+        <f>U371/U370</f>
+        <v>1.8345323741007041E-2</v>
+      </c>
+      <c r="V372">
+        <f>U372*4</f>
+        <v>7.3381294964028163E-2</v>
+      </c>
+      <c r="W372">
+        <f>1/U372</f>
+        <v>54.50980392156908</v>
+      </c>
+    </row>
+    <row r="373" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C373">
         <v>446</v>
       </c>
@@ -40282,7 +40943,7 @@
         <v>2.2299999999999998E-6</v>
       </c>
     </row>
-    <row r="374" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="374" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C374">
         <v>447</v>
       </c>
@@ -40310,8 +40971,40 @@
         <f t="shared" si="46"/>
         <v>2.2349999999999998E-6</v>
       </c>
-    </row>
-    <row r="375" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N374" t="s">
+        <v>167</v>
+      </c>
+      <c r="O374" t="s">
+        <v>173</v>
+      </c>
+      <c r="P374" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q374" t="s">
+        <v>117</v>
+      </c>
+      <c r="R374" t="s">
+        <v>166</v>
+      </c>
+      <c r="S374">
+        <v>1.3649</v>
+      </c>
+      <c r="T374">
+        <v>1.9846999999999999</v>
+      </c>
+      <c r="U374">
+        <f>T374-S374</f>
+        <v>0.61979999999999991</v>
+      </c>
+      <c r="V374">
+        <f>1/U374</f>
+        <v>1.613423685059697</v>
+      </c>
+      <c r="W374" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="375" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C375">
         <v>448</v>
       </c>
@@ -40339,8 +41032,21 @@
         <f t="shared" si="46"/>
         <v>2.2400000000000002E-6</v>
       </c>
-    </row>
-    <row r="376" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="N375" t="s">
+        <v>162</v>
+      </c>
+      <c r="S375">
+        <v>1.3920999999999999</v>
+      </c>
+      <c r="T375">
+        <v>1.4058999999999999</v>
+      </c>
+      <c r="U375">
+        <f>T375-S375</f>
+        <v>1.3800000000000034E-2</v>
+      </c>
+    </row>
+    <row r="376" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C376">
         <v>449</v>
       </c>
@@ -40368,8 +41074,20 @@
         <f t="shared" si="46"/>
         <v>2.2450000000000001E-6</v>
       </c>
-    </row>
-    <row r="377" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="U376">
+        <f>U375/U374</f>
+        <v>2.2265246853823872E-2</v>
+      </c>
+      <c r="V376">
+        <f>U376*4</f>
+        <v>8.9060987415295487E-2</v>
+      </c>
+      <c r="W376">
+        <f>1/U376</f>
+        <v>44.913043478260754</v>
+      </c>
+    </row>
+    <row r="377" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C377">
         <v>450</v>
       </c>
@@ -40398,7 +41116,7 @@
         <v>2.2500000000000001E-6</v>
       </c>
     </row>
-    <row r="378" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="378" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C378">
         <v>451</v>
       </c>
@@ -40427,7 +41145,7 @@
         <v>2.255E-6</v>
       </c>
     </row>
-    <row r="379" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="379" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C379">
         <v>452</v>
       </c>
@@ -40456,7 +41174,7 @@
         <v>2.26E-6</v>
       </c>
     </row>
-    <row r="380" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="380" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C380">
         <v>453</v>
       </c>
@@ -40485,7 +41203,7 @@
         <v>2.2649999999999999E-6</v>
       </c>
     </row>
-    <row r="381" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="381" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C381">
         <v>454</v>
       </c>
@@ -40514,7 +41232,7 @@
         <v>2.2699999999999999E-6</v>
       </c>
     </row>
-    <row r="382" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="382" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C382">
         <v>455</v>
       </c>
@@ -40543,7 +41261,7 @@
         <v>2.2750000000000002E-6</v>
       </c>
     </row>
-    <row r="383" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="383" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C383">
         <v>456</v>
       </c>
@@ -40572,7 +41290,7 @@
         <v>2.2800000000000002E-6</v>
       </c>
     </row>
-    <row r="384" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="384" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C384">
         <v>457</v>
       </c>
@@ -51132,4 +51850,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>